<commit_message>
fix various publishing issues pre-apply FHIR-27862 and FHIR-27818
</commit_message>
<xml_diff>
--- a/temp/StructureDefinition-indv-measurereport-deqm.xlsx
+++ b/temp/StructureDefinition-indv-measurereport-deqm.xlsx
@@ -5713,7 +5713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
         <v>248</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>46</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>38</v>

</xml_diff>